<commit_message>
Merge branches 'master' and 'PROS-5326-ccru-premium-spirits-picos' of bitbucket.org:traxtechnology/kpi_factory into PROS-5326-ccru-premium-spirits-picos
# Conflicts:
#	Projects/CCRU/Utils/TopSKU.py
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Spirits 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Spirits 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -188,12 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">Чинзано Бьянко - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cinzano Bianco - 1.0L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Чинзано Бьянко - 1.0л</t>
   </si>
   <si>
     <t xml:space="preserve">Old Smuggler - 0.7L</t>
@@ -262,7 +256,10 @@
     <t xml:space="preserve">Кампари Дисплей</t>
   </si>
   <si>
-    <t xml:space="preserve">Manufacture: CAMPARI</t>
+    <t xml:space="preserve">Manufacturer: CAMPARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN</t>
   </si>
   <si>
     <t xml:space="preserve">Display Alcohol</t>
@@ -280,7 +277,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -303,15 +300,8 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,18 +310,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -339,23 +323,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,11 +348,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,12 +370,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -420,84 +382,23 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF9C5700"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -506,35 +407,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="31.45"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="19" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.0607287449393"/>
     <col collapsed="false" hidden="false" max="28" min="24" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -656,7 +561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
@@ -703,7 +608,7 @@
         <v>51</v>
       </c>
       <c r="AC2" s="5" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="AJ2" s="0" t="n">
         <v>2</v>
@@ -712,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
@@ -758,8 +663,8 @@
       <c r="AB3" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="6" t="n">
-        <v>0.12</v>
+      <c r="AC3" s="5" t="n">
+        <v>0.18</v>
       </c>
       <c r="AJ3" s="0" t="n">
         <v>2</v>
@@ -768,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
@@ -814,8 +719,8 @@
       <c r="AB4" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="AC4" s="6" t="n">
-        <v>0.07</v>
+      <c r="AC4" s="5" t="n">
+        <v>0.1</v>
       </c>
       <c r="AJ4" s="0" t="n">
         <v>2</v>
@@ -824,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
@@ -847,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>8000020000013</v>
+        <v>5010327605005</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>45</v>
@@ -870,17 +775,17 @@
       <c r="AB5" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="AC5" s="6" t="n">
+      <c r="AC5" s="5" t="n">
         <v>0.07</v>
       </c>
       <c r="AJ5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
@@ -900,43 +805,44 @@
         <v>44</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>5010327605005</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="K6" s="0"/>
       <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="N6" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="O6" s="0" t="s">
         <v>46</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="AA6" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC6" s="6" t="n">
-        <v>0.09</v>
+        <v>64</v>
+      </c>
+      <c r="AC6" s="5" t="n">
+        <v>0.15</v>
       </c>
       <c r="AJ6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
@@ -947,53 +853,55 @@
         <v>41</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K7" s="0"/>
+        <v>6</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>8000020000280</v>
+      </c>
       <c r="L7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="O7" s="0" t="s">
         <v>46</v>
       </c>
       <c r="P7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="AA7" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC7" s="2" t="n">
-        <v>0.2</v>
+        <v>64</v>
+      </c>
+      <c r="AC7" s="5" t="n">
+        <v>0.15</v>
       </c>
       <c r="AJ7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK7" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
@@ -1004,22 +912,22 @@
         <v>41</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="8" t="n">
-        <v>8000020000280</v>
+      <c r="G8" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>45</v>
@@ -1031,28 +939,28 @@
         <v>47</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA8" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC8" s="2" t="n">
-        <v>0.1</v>
+        <v>64</v>
+      </c>
+      <c r="AC8" s="5" t="n">
+        <v>0.05</v>
       </c>
       <c r="AJ8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK8" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
@@ -1063,55 +971,52 @@
         <v>41</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="N9" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="O9" s="0" t="s">
         <v>46</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA9" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC9" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="AC9" s="5" t="n">
         <v>0.05</v>
       </c>
       <c r="AJ9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK9" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
@@ -1122,115 +1027,57 @@
         <v>41</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K10" s="0"/>
+        <v>8</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>77</v>
+      </c>
       <c r="L10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>76</v>
-      </c>
       <c r="O10" s="0" t="s">
         <v>46</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="U10" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="W10" s="0" t="s">
-        <v>65</v>
+        <v>78</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>79</v>
       </c>
       <c r="AA10" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC10" s="2" t="n">
-        <v>0.1</v>
+        <v>51</v>
+      </c>
+      <c r="AC10" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="AJ10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AK10" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="V11" s="0" t="s">
+    <row r="13" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M13" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="AA11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK11" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M14" s="0" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
PROS-5201 - CCRU Spirits update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Spirits 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Spirits 2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -410,30 +410,30 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.45"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="19" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.0607287449393"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.3846153846154"/>
     <col collapsed="false" hidden="false" max="28" min="24" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.57085020242915"/>
@@ -807,7 +807,9 @@
       <c r="G6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="0"/>
+      <c r="K6" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
@@ -982,6 +984,9 @@
       <c r="G9" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="K9" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="L9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1040,6 +1045,9 @@
       </c>
       <c r="J10" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>45</v>

</xml_diff>